<commit_message>
update topic selection and project 3 group
</commit_message>
<xml_diff>
--- a/P2/P2_PeerReview.xlsx
+++ b/P2/P2_PeerReview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TTU-CS\Github\CS5331_Spring2019\P2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3EDF8B-910A-4A2F-99E9-07DDD0B8FAD7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC6F711-CCCE-4405-A01C-6C1716492F74}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{5E94E157-D904-4DD4-8FF9-3E443BED4110}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Group</t>
   </si>
@@ -290,6 +290,14 @@
 Excellent coding proficiency and communication. A good team player.
 Nhat: 5
 Helpful insight and project commitment. Good communication and professionalism.</t>
+  </si>
+  <si>
+    <t>Elizabeth Doyle
+5
+Elizabeth was a wonderful partner for the second project. Although she was also very busy, she put a lot of work and effort into the project. Elizabeth did a great job with the co-occurrence matrix on the project.
+Matthew Hendrick
+5
+Matt did a great job with the initial data retrieval and setup. He spent a lot of time on writing java programs to pre-process the data for what we needed in the project. Matt’s contribution was definitely needed for the project to be successful.</t>
   </si>
 </sst>
 </file>
@@ -646,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E895BF0F-A436-4AA9-BB43-4FAEB3E2D715}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,12 +861,15 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>